<commit_message>
Finished analysis of expert group
</commit_message>
<xml_diff>
--- a/datasets/expertgroup/dataset_expertgroup.xlsx
+++ b/datasets/expertgroup/dataset_expertgroup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\AMS\Thesis\datasets\expertgroup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rblieken\Dropbox\MacWinSwap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4938780-BA83-4F24-861B-37766266773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CB7B3D-B0EC-4634-A986-3FEF6F14FB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Validation of Succes Factors EA" sheetId="1" r:id="rId1"/>
@@ -30,16 +30,18 @@
     <sheet name="To what extent are the attrib 1" sheetId="13" r:id="rId15"/>
     <sheet name="Scoring EA" sheetId="20" r:id="rId16"/>
     <sheet name="End Survey Flipboard" sheetId="14" r:id="rId17"/>
-    <sheet name="End Survey" sheetId="15" r:id="rId18"/>
-    <sheet name="Follow up list" sheetId="16" r:id="rId19"/>
-    <sheet name="Follow up voting" sheetId="17" r:id="rId20"/>
-    <sheet name="Wrap up" sheetId="18" r:id="rId21"/>
+    <sheet name="Charts end survey" sheetId="24" r:id="rId18"/>
+    <sheet name="End Survey" sheetId="15" r:id="rId19"/>
+    <sheet name="Follow up list" sheetId="16" r:id="rId20"/>
+    <sheet name="Follow up voting" sheetId="17" r:id="rId21"/>
+    <sheet name="Wrap up" sheetId="18" r:id="rId22"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId22"/>
-    <pivotCache cacheId="10" r:id="rId23"/>
-    <pivotCache cacheId="14" r:id="rId24"/>
+    <pivotCache cacheId="0" r:id="rId23"/>
+    <pivotCache cacheId="1" r:id="rId24"/>
+    <pivotCache cacheId="2" r:id="rId25"/>
+    <pivotCache cacheId="8" r:id="rId26"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="137">
   <si>
     <t>Title</t>
   </si>
@@ -857,7 +859,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796856"/>
@@ -917,7 +919,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796528"/>
@@ -959,7 +961,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -995,7 +997,7 @@
           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1081,7 +1083,7 @@
                     <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1264,7 +1266,7 @@
                           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                         </a:defRPr>
                       </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
+                      <a:endParaRPr lang="nl-NL"/>
                     </a:p>
                   </c:txPr>
                   <c:dLblPos val="outEnd"/>
@@ -1445,7 +1447,7 @@
                           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                         </a:defRPr>
                       </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
+                      <a:endParaRPr lang="nl-NL"/>
                     </a:p>
                   </c:txPr>
                   <c:dLblPos val="outEnd"/>
@@ -1610,7 +1612,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796856"/>
@@ -1693,7 +1695,7 @@
                   <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1725,7 +1727,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796528"/>
@@ -1764,7 +1766,7 @@
           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1850,7 +1852,7 @@
                     <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1977,7 +1979,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796856"/>
@@ -2059,7 +2061,7 @@
                   <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2091,7 +2093,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796528"/>
@@ -2130,7 +2132,7 @@
           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2326,7 +2328,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796856"/>
@@ -2386,7 +2388,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796528"/>
@@ -2428,7 +2430,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -2464,7 +2466,7 @@
           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2550,7 +2552,7 @@
                     <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2731,7 +2733,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796856"/>
@@ -2814,7 +2816,7 @@
                   <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="nl-NL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2846,7 +2848,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796528"/>
@@ -2885,7 +2887,7 @@
           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3077,7 +3079,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796856"/>
@@ -3137,7 +3139,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="573796528"/>
@@ -3179,7 +3181,7 @@
                 <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
       </c:dTable>
@@ -3221,7 +3223,338 @@
           <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="101"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="1"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:clrMapOvr bg1="lt1" tx1="dk1" bg2="lt2" tx2="dk2" accent1="accent1" accent2="accent2" accent3="accent3" accent4="accent4" accent5="accent5" accent6="accent6" hlink="hlink" folHlink="folHlink"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Charts end survey'!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rating</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:tint val="88500"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Charts end survey'!$B$9:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Participant C</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Participant E</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Participant H</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Participant J</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Participant A</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Participant D</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Participant G</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Participant B</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Participant F</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Participant I</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Charts end survey'!$C$9:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3FB9-4E39-B4C9-00E922181E06}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="573796528"/>
+        <c:axId val="573796856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="573796528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573796856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="573796856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="573796528"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="0"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:ea typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+                <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nl-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+          <a:cs typeface="CMU Sans Serif" panose="02000603000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3394,6 +3727,33 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5910,6 +6270,509 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6658,6 +7521,47 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>358773</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>377673</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>2250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2C602DE-C5B0-D389-4348-DCAF23A51674}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Bliekendaal, Rene" refreshedDate="44675.861565740743" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="120" xr:uid="{1B10E4F2-E95C-46D3-AD52-8DFE19CDBF70}">
   <cacheSource type="worksheet">
@@ -6796,6 +7700,47 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Bliekendaal, Rene" refreshedDate="44688.652495949071" createdVersion="7" refreshedVersion="7" minRefreshableVersion="3" recordCount="50" xr:uid="{D3A7DBD3-ABBF-4A11-9048-AE293AC9B715}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A8:C58" sheet="End Survey"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Item" numFmtId="0">
+      <sharedItems count="5">
+        <s v="To what extent do you find the research relevant?"/>
+        <s v="To what extent did this session fulfil your expectations?"/>
+        <s v="To what extent do you think that the research can be used by yourself?"/>
+        <s v="To what extent do you think that the research can be used in the public sector?"/>
+        <s v="To what extent do you think that the research can be used by your organisation?"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Rating" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="10"/>
+    </cacheField>
+    <cacheField name="Name" numFmtId="0">
+      <sharedItems count="10">
+        <s v="Participant A"/>
+        <s v="Participant J"/>
+        <s v="Participant D"/>
+        <s v="Participant C"/>
+        <s v="Participant G"/>
+        <s v="Participant F"/>
+        <s v="Participant I"/>
+        <s v="Participant E"/>
+        <s v="Participant H"/>
+        <s v="Participant B"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="120">
   <r>
@@ -8161,8 +9106,263 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="50">
+  <r>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="9"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="9"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="10"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="9"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="8"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="10"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="9"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="9"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="7"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="7"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="7"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="9"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="7"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="4"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="9"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="6"/>
+    <x v="9"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="8"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="8"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="8"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="6"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="4"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="8"/>
+    <x v="8"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="6"/>
+    <x v="9"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF9132D4-8EDD-4ECF-9C0E-B2A4F7955B7E}" name="PivotTable3" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF9132D4-8EDD-4ECF-9C0E-B2A4F7955B7E}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:N6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -8261,7 +9461,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C64600C-59D3-4441-9C7A-3587AAEA11F7}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C64600C-59D3-4441-9C7A-3587AAEA11F7}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:N6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -8355,7 +9555,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63E50793-E8F1-4A14-B209-2D078243FA14}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{63E50793-E8F1-4A14-B209-2D078243FA14}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="C3:N6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -8444,6 +9644,101 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Rating" fld="1" baseField="0" baseItem="2010282276"/>
+  </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B0E9A131-3FB0-441D-9A36-4A94016CC04B}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:L6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item h="1" x="1"/>
+        <item h="1" x="0"/>
+        <item h="1" x="4"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item x="9"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="8"/>
+        <item x="6"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="2">
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="2"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Rating" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -10147,11 +11442,292 @@
 </a:themeOverride>
 </file>
 
+<file path=xl/theme/themeOverride6.xml><?xml version="1.0" encoding="utf-8"?>
+<a:themeOverride xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <a:clrScheme name="Office">
+    <a:dk1>
+      <a:sysClr val="windowText" lastClr="000000"/>
+    </a:dk1>
+    <a:lt1>
+      <a:sysClr val="window" lastClr="FFFFFF"/>
+    </a:lt1>
+    <a:dk2>
+      <a:srgbClr val="1F497D"/>
+    </a:dk2>
+    <a:lt2>
+      <a:srgbClr val="EEECE1"/>
+    </a:lt2>
+    <a:accent1>
+      <a:srgbClr val="4F81BD"/>
+    </a:accent1>
+    <a:accent2>
+      <a:srgbClr val="C0504D"/>
+    </a:accent2>
+    <a:accent3>
+      <a:srgbClr val="9BBB59"/>
+    </a:accent3>
+    <a:accent4>
+      <a:srgbClr val="8064A2"/>
+    </a:accent4>
+    <a:accent5>
+      <a:srgbClr val="4BACC6"/>
+    </a:accent5>
+    <a:accent6>
+      <a:srgbClr val="F79646"/>
+    </a:accent6>
+    <a:hlink>
+      <a:srgbClr val="0000FF"/>
+    </a:hlink>
+    <a:folHlink>
+      <a:srgbClr val="800080"/>
+    </a:folHlink>
+  </a:clrScheme>
+  <a:fontScheme name="Office">
+    <a:majorFont>
+      <a:latin typeface="Cambria"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Times New Roman"/>
+      <a:font script="Hebr" typeface="Times New Roman"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="MoolBoran"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Times New Roman"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:majorFont>
+    <a:minorFont>
+      <a:latin typeface="Calibri"/>
+      <a:ea typeface=""/>
+      <a:cs typeface=""/>
+      <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+      <a:font script="Hang" typeface="맑은 고딕"/>
+      <a:font script="Hans" typeface="宋体"/>
+      <a:font script="Hant" typeface="新細明體"/>
+      <a:font script="Arab" typeface="Arial"/>
+      <a:font script="Hebr" typeface="Arial"/>
+      <a:font script="Thai" typeface="Tahoma"/>
+      <a:font script="Ethi" typeface="Nyala"/>
+      <a:font script="Beng" typeface="Vrinda"/>
+      <a:font script="Gujr" typeface="Shruti"/>
+      <a:font script="Khmr" typeface="DaunPenh"/>
+      <a:font script="Knda" typeface="Tunga"/>
+      <a:font script="Guru" typeface="Raavi"/>
+      <a:font script="Cans" typeface="Euphemia"/>
+      <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+      <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+      <a:font script="Thaa" typeface="MV Boli"/>
+      <a:font script="Deva" typeface="Mangal"/>
+      <a:font script="Telu" typeface="Gautami"/>
+      <a:font script="Taml" typeface="Latha"/>
+      <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+      <a:font script="Orya" typeface="Kalinga"/>
+      <a:font script="Mlym" typeface="Kartika"/>
+      <a:font script="Laoo" typeface="DokChampa"/>
+      <a:font script="Sinh" typeface="Iskoola Pota"/>
+      <a:font script="Mong" typeface="Mongolian Baiti"/>
+      <a:font script="Viet" typeface="Arial"/>
+      <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      <a:font script="Geor" typeface="Sylfaen"/>
+    </a:minorFont>
+  </a:fontScheme>
+  <a:fmtScheme name="Office">
+    <a:fillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="50000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="35000">
+            <a:schemeClr val="phClr">
+              <a:tint val="37000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:tint val="15000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="1"/>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:shade val="51000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="80000">
+            <a:schemeClr val="phClr">
+              <a:shade val="93000"/>
+              <a:satMod val="130000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="94000"/>
+              <a:satMod val="135000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:lin ang="16200000" scaled="0"/>
+      </a:gradFill>
+    </a:fillStyleLst>
+    <a:lnStyleLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:shade val="95000"/>
+            <a:satMod val="105000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+      <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="solid"/>
+      </a:ln>
+    </a:lnStyleLst>
+    <a:effectStyleLst>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:effectStyle>
+      <a:effectStyle>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="threePt" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="63500" h="25400"/>
+        </a:sp3d>
+      </a:effectStyle>
+    </a:effectStyleLst>
+    <a:bgFillStyleLst>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="40000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="40000">
+            <a:schemeClr val="phClr">
+              <a:tint val="45000"/>
+              <a:shade val="99000"/>
+              <a:satMod val="350000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="20000"/>
+              <a:satMod val="255000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+      </a:gradFill>
+      <a:gradFill rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="phClr">
+              <a:tint val="80000"/>
+              <a:satMod val="300000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="phClr">
+              <a:shade val="30000"/>
+              <a:satMod val="200000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+    </a:bgFillStyleLst>
+  </a:fmtScheme>
+</a:themeOverride>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -13705,7 +15281,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -13755,11 +15331,257 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DED03F0-0E08-4C03-8423-4E6789AB7336}">
+  <dimension ref="A3:L18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="67.23046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3828125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.61328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.4609375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.61328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.69140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" s="11">
+        <v>7</v>
+      </c>
+      <c r="C5" s="12">
+        <v>6</v>
+      </c>
+      <c r="D5" s="12">
+        <v>9</v>
+      </c>
+      <c r="E5" s="12">
+        <v>7</v>
+      </c>
+      <c r="F5" s="12">
+        <v>9</v>
+      </c>
+      <c r="G5" s="12">
+        <v>4</v>
+      </c>
+      <c r="H5" s="12">
+        <v>7</v>
+      </c>
+      <c r="I5" s="12">
+        <v>8</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12">
+        <v>8</v>
+      </c>
+      <c r="L5" s="13">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="14">
+        <v>7</v>
+      </c>
+      <c r="C6" s="15">
+        <v>6</v>
+      </c>
+      <c r="D6" s="15">
+        <v>9</v>
+      </c>
+      <c r="E6" s="15">
+        <v>7</v>
+      </c>
+      <c r="F6" s="15">
+        <v>9</v>
+      </c>
+      <c r="G6" s="15">
+        <v>4</v>
+      </c>
+      <c r="H6" s="15">
+        <v>7</v>
+      </c>
+      <c r="I6" s="15">
+        <v>8</v>
+      </c>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15">
+        <v>8</v>
+      </c>
+      <c r="L6" s="16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B9" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C16" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="12"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B9:C18">
+    <sortCondition descending="1" ref="C9:C18"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -14434,45 +16256,6 @@
       </c>
       <c r="C58" t="s">
         <v>114</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="66.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -14656,10 +16439,51 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="66.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -14955,7 +16779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -16479,7 +18303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>